<commit_message>
updated  created date in Group.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Group.xlsx
+++ b/Design Data/Sample Data/Excel Files/Group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F09BBB-2F93-4F13-998E-9FC244053013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2625A5BF-F5EB-4681-A95F-087BF6591C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -94,6 +94,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,7 +381,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -395,7 +399,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
@@ -406,36 +410,64 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C5" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="3">
+        <v>44075</v>
+      </c>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated last edited in Group.xlsx
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Group.xlsx
+++ b/Design Data/Sample Data/Excel Files/Group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2625A5BF-F5EB-4681-A95F-087BF6591C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A86FC-6F7F-4AE2-A48E-CB81F7D345B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -97,7 +97,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,9 +379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -402,7 +399,7 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -413,7 +410,9 @@
       <c r="C2" s="3">
         <v>44075</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -422,7 +421,9 @@
       <c r="C3" s="3">
         <v>44075</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -431,7 +432,9 @@
       <c r="C4" s="3">
         <v>44075</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
@@ -440,7 +443,9 @@
       <c r="C5" s="3">
         <v>44075</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -449,7 +454,9 @@
       <c r="C6" s="3">
         <v>44075</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
@@ -458,7 +465,9 @@
       <c r="C7" s="3">
         <v>44075</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="3">
+        <v>44091</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
@@ -467,7 +476,9 @@
       <c r="C8" s="3">
         <v>44075</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3">
+        <v>44091</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>